<commit_message>
schedule-equipo ciclo1 y 2
</commit_message>
<xml_diff>
--- a/NoteBook/summary/SCHEDULE_TEAM.xlsx
+++ b/NoteBook/summary/SCHEDULE_TEAM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\tsp\NoteBook\summary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="19980" windowHeight="7815"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>TSPi Schedule Planning Template - Form SCHEDULE</t>
   </si>
@@ -73,6 +78,9 @@
   </si>
   <si>
     <t>12/03/214</t>
+  </si>
+  <si>
+    <t>16/024/2014</t>
   </si>
 </sst>
 </file>
@@ -295,6 +303,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -305,6 +325,84 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,96 +410,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,6 +420,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -460,7 +471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,7 +506,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,14 +732,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -751,209 +762,209 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="13" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14">
+      <c r="I3" s="43"/>
+      <c r="J3" s="44">
         <v>41719</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="13" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="16" t="s">
+      <c r="I4" s="43"/>
+      <c r="J4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="13" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="16">
+      <c r="I5" s="43"/>
+      <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="43" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="43" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="10" t="s">
+      <c r="H8" s="33"/>
+      <c r="I8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="10" t="s">
+      <c r="K8" s="33"/>
+      <c r="L8" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>1</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="8">
         <v>17.5</v>
       </c>
@@ -964,17 +975,17 @@
       <c r="F14" s="9">
         <v>11.6</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="27">
         <v>17.5</v>
       </c>
-      <c r="H14" s="18"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="8">
         <v>17.5</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="27">
         <v>11.6</v>
       </c>
-      <c r="K14" s="18"/>
+      <c r="K14" s="28"/>
       <c r="L14" s="8">
         <f>J14</f>
         <v>11.6</v>
@@ -984,10 +995,10 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="31">
         <v>41717</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="9">
         <v>0</v>
       </c>
@@ -998,18 +1009,18 @@
       <c r="F15" s="9">
         <v>11.6</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="27">
         <v>0</v>
       </c>
-      <c r="H15" s="18"/>
+      <c r="H15" s="28"/>
       <c r="I15" s="9">
         <f>G15+I14</f>
         <v>17.5</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="27">
         <v>0</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="K15" s="28"/>
       <c r="L15" s="9">
         <f>J15+L14</f>
         <v>11.6</v>
@@ -1019,10 +1030,10 @@
       <c r="A16" s="5">
         <v>3</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="31">
         <v>41724</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="9">
         <v>41</v>
       </c>
@@ -1033,18 +1044,18 @@
       <c r="F16" s="9">
         <v>39</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="27">
         <v>38</v>
       </c>
-      <c r="H16" s="18"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="9">
         <f>G16+I15</f>
         <v>55.5</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="27">
         <v>27.4</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="28"/>
       <c r="L16" s="9">
         <f>J16+L15</f>
         <v>39</v>
@@ -1054,10 +1065,10 @@
       <c r="A17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="31">
         <v>41731</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="9">
         <v>26.5</v>
       </c>
@@ -1068,21 +1079,31 @@
       <c r="F17" s="9">
         <v>56.6</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="9"/>
+      <c r="G17" s="27">
+        <v>31.4</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="9">
+        <f t="shared" ref="I17:I19" si="1">G17+I16</f>
+        <v>86.9</v>
+      </c>
+      <c r="J17" s="27">
+        <v>14.6</v>
+      </c>
+      <c r="K17" s="28"/>
+      <c r="L17" s="9">
+        <f t="shared" ref="L17:L19" si="2">J17+L16</f>
+        <v>53.6</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>5</v>
       </c>
-      <c r="B18" s="17">
-        <v>41679</v>
-      </c>
-      <c r="C18" s="18"/>
+      <c r="B18" s="31">
+        <v>41738</v>
+      </c>
+      <c r="C18" s="28"/>
       <c r="D18" s="9">
         <v>53</v>
       </c>
@@ -1093,21 +1114,31 @@
       <c r="F18" s="9">
         <v>91.7</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="9"/>
+      <c r="G18" s="27">
+        <v>59.7</v>
+      </c>
+      <c r="H18" s="28"/>
+      <c r="I18" s="9">
+        <f t="shared" si="1"/>
+        <v>146.60000000000002</v>
+      </c>
+      <c r="J18" s="27">
+        <v>29.5</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="9">
+        <f t="shared" si="2"/>
+        <v>83.1</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>6</v>
       </c>
-      <c r="B19" s="17">
-        <v>41686</v>
-      </c>
-      <c r="C19" s="18"/>
+      <c r="B19" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="28"/>
       <c r="D19" s="9">
         <v>12.5</v>
       </c>
@@ -1118,29 +1149,76 @@
       <c r="F19" s="9">
         <v>100</v>
       </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="9"/>
+      <c r="G19" s="27">
+        <v>40.4</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="9">
+        <f t="shared" si="1"/>
+        <v>187.00000000000003</v>
+      </c>
+      <c r="J19" s="27">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="L19" s="9">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="33"/>
+      <c r="G20" s="29">
+        <f>SUM(G14:H19)</f>
+        <v>187.00000000000003</v>
+      </c>
+      <c r="H20" s="30"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33"/>
+      <c r="J20" s="29">
+        <f>SUM(J14:K19)</f>
+        <v>100</v>
+      </c>
+      <c r="K20" s="30"/>
       <c r="L20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J8:K13"/>
+    <mergeCell ref="B8:C13"/>
+    <mergeCell ref="G8:H13"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J19:K19"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="D8:D13"/>
@@ -1157,37 +1235,6 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J8:K13"/>
-    <mergeCell ref="B8:C13"/>
-    <mergeCell ref="G8:H13"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>